<commit_message>
Refactor forecasting logic in tc.py to implement stricter confidence interval limits and improve visualization transitions. Remove temporary Excel file and update comments for clarity. Add error handling in tr.py for data loading and processing.
</commit_message>
<xml_diff>
--- a/Travelicious Restaurant Data.xlsx
+++ b/Travelicious Restaurant Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tothemoon/Clients/Travelicious and Travellers Cavern/Business Forecasting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EBD8FD-0BCF-AA41-9103-F8F3A2D41A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822F8DFA-32CB-704B-AA80-A1E1C5770B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15580" xr2:uid="{A9F63F80-A1D0-6A44-B225-19EFC06B72B6}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -81,12 +81,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Abadi Extra Light"/>
+      <name val="Aptos Display"/>
+      <scheme val="major"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Abadi Extra Light"/>
+      <name val="Aptos Display"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Display"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="6">
@@ -154,25 +162,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="17" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -512,7 +520,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -528,7 +536,7 @@
     <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>